<commit_message>
cabmios para el deploy
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ihour\Desktop\repos\renova\renova-product-quotator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3D91F0-F374-40A4-883B-AEC6F03A7F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{541FE9FF-E291-4642-AEA9-443F9F41A825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -206,19 +206,19 @@
     <t>https://www.dhfdistribuidora.com.ar/content/bucket/1/2041w430h270.jpg.webp</t>
   </si>
   <si>
-    <t>https://catalogofram.com.ar/img?url=https%3A%2F%2Fproduction-specparts-search-api-images-bucket.s3.amazonaws.com%2Fpart_pictures%2FodkNrJ4jaRJKup4uPYeuJpZpCthCCoiM.jpg</t>
-  </si>
-  <si>
     <t>https://catalogofram.com.ar/img?url=https%3A%2F%2Fproduction-specparts-search-api-images-bucket.s3.amazonaws.com%2Fpart_pictures%2FU8AMrhqlgiWkp3zCk7exfo5uMQOMaTq3.jpg</t>
   </si>
   <si>
     <t>https://i2.wp.com/tuautoideal.com.ar/wp-content/uploads/2022/04/argo-drive-grande1-1.jpg?zoom=1.25&amp;fit=1113%2C1113&amp;ssl=1</t>
   </si>
   <si>
-    <t>https://catalogofram.com.ar/img?url=https%3A%2F%2Fproduction-specparts-search-api-images-bucket.s3.amazonaws.com%2Fpart_pictures%2FOvRXIBulkwgiUGaBOQETtmseIu305iY2.jpg</t>
-  </si>
-  <si>
-    <t>https://catalogofram.com.ar/img?url=https%3A%2F%2Fproduction-specparts-search-api-images-bucket.s3.amazonaws.com%2Fpart_pictures%2F2liwqz8LkCYWhh9okVOo6E8PsHXpbrEq.jpg</t>
+    <t>https://http2.mlstatic.com/D_NQ_NP_2X_881694-MLA70061350186_062023-F.webp</t>
+  </si>
+  <si>
+    <t>https://http2.mlstatic.com/D_NQ_NP_2X_815627-MLA72720301527_112023-F.webp</t>
+  </si>
+  <si>
+    <t>https://http2.mlstatic.com/D_NQ_NP_2X_680318-MLA75641583430_042024-F.webp</t>
   </si>
 </sst>
 </file>
@@ -785,7 +785,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
         <v>52</v>
@@ -816,7 +816,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -969,7 +969,7 @@
         <v>45</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
         <v>29</v>
@@ -997,7 +997,7 @@
         <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
         <v>35</v>
@@ -1011,7 +1011,7 @@
         <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>

</xml_diff>